<commit_message>
Changed SkillLevelConfig to use enum instead of string for AttributeType
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__beans__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__beans__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignData\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC37272-9D90-4D7C-A59B-45C6946B467C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE7F65C-C04E-4A35-8CEF-673DFDB67DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="870" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>##var</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>attributeType</t>
+  </si>
+  <si>
+    <t>AttributeType</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -209,9 +212,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -493,7 +493,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -602,19 +602,19 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="H6" s="5" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>19</v>
+      <c r="I6" t="s">
+        <v>26</v>
       </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="H7" s="5" t="s">
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="2"/>

</xml_diff>

<commit_message>
Made SkillManager be able to use SkillConfig
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__beans__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__beans__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE7F65C-C04E-4A35-8CEF-673DFDB67DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BE0F38-CE6B-4C12-840A-9DABE0CB1780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="870" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>##var</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>AttributeType</t>
+  </si>
+  <si>
+    <t>AttributeTypeAndFloat</t>
   </si>
 </sst>
 </file>
@@ -493,12 +496,13 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="7" width="15" customWidth="1"/>
     <col min="8" max="9" width="13.42578125" customWidth="1"/>
@@ -620,7 +624,23 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" s="3"/>

</xml_diff>